<commit_message>
The excel parser now works.
</commit_message>
<xml_diff>
--- a/Documents/Research/DART I3 - Safe Braking Distance -SBD Calculations_1_29_2014_Change Per C....xlsx
+++ b/Documents/Research/DART I3 - Safe Braking Distance -SBD Calculations_1_29_2014_Change Per C....xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ZacharyDesktop\Documents\GitHub\SeniorProj\Documents\Research\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Chad\Documents\SeniorProj\Documents\Research\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -1299,16 +1299,6 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1" indent="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1341,6 +1331,16 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="5">
@@ -1657,8 +1657,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AF72"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="81" zoomScaleNormal="81" workbookViewId="0">
-      <selection activeCell="S4" sqref="S4"/>
+    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="81" zoomScaleNormal="81" workbookViewId="0">
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1761,9 +1761,9 @@
       <c r="AA4" s="19"/>
       <c r="AB4" s="18"/>
       <c r="AC4" s="18"/>
-      <c r="AD4" s="91"/>
-      <c r="AE4" s="84"/>
-      <c r="AF4" s="84"/>
+      <c r="AD4" s="87"/>
+      <c r="AE4" s="80"/>
+      <c r="AF4" s="80"/>
     </row>
     <row r="5" spans="1:32" s="1" customFormat="1" ht="13.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B5" s="2" t="s">
@@ -1850,7 +1850,7 @@
       <c r="AC5" s="17" t="s">
         <v>60</v>
       </c>
-      <c r="AD5" s="92" t="s">
+      <c r="AD5" s="88" t="s">
         <v>69</v>
       </c>
       <c r="AE5" s="79"/>
@@ -1938,14 +1938,14 @@
       <c r="AB6" s="11" t="s">
         <v>53</v>
       </c>
-      <c r="AC6" s="88" t="s">
+      <c r="AC6" s="84" t="s">
         <v>28</v>
       </c>
-      <c r="AD6" s="93" t="s">
+      <c r="AD6" s="89" t="s">
         <v>29</v>
       </c>
-      <c r="AE6" s="85"/>
-      <c r="AF6" s="85"/>
+      <c r="AE6" s="81"/>
+      <c r="AF6" s="81"/>
     </row>
     <row r="7" spans="1:32" s="1" customFormat="1" ht="25.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B7" s="18">
@@ -2037,15 +2037,15 @@
         <f>P7+U7+W7+Y7+R7+Z7</f>
         <v>344.78218755953947</v>
       </c>
-      <c r="AC7" s="89">
+      <c r="AC7" s="85">
         <f t="shared" ref="AC7:AC17" si="0">H7-AB7</f>
         <v>245.21781244046053</v>
       </c>
-      <c r="AD7" s="94" t="s">
+      <c r="AD7" s="90" t="s">
         <v>30</v>
       </c>
-      <c r="AE7" s="86"/>
-      <c r="AF7" s="87"/>
+      <c r="AE7" s="82"/>
+      <c r="AF7" s="83"/>
     </row>
     <row r="8" spans="1:32" s="1" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B8" s="18"/>
@@ -2131,11 +2131,11 @@
         <f t="shared" ref="AB8:AB17" si="10">P8+U8+W8+Y8+R8+Z8</f>
         <v>943.37860768880705</v>
       </c>
-      <c r="AC8" s="89">
+      <c r="AC8" s="85">
         <f t="shared" si="0"/>
         <v>261.62139231119295</v>
       </c>
-      <c r="AD8" s="94" t="s">
+      <c r="AD8" s="90" t="s">
         <v>30</v>
       </c>
       <c r="AE8" s="4"/>
@@ -2231,11 +2231,11 @@
         <f t="shared" si="10"/>
         <v>436.23582300230191</v>
       </c>
-      <c r="AC9" s="89">
+      <c r="AC9" s="85">
         <f t="shared" si="0"/>
         <v>178.76417699769809</v>
       </c>
-      <c r="AD9" s="94" t="s">
+      <c r="AD9" s="90" t="s">
         <v>30</v>
       </c>
       <c r="AE9" s="4"/>
@@ -2325,11 +2325,11 @@
         <f t="shared" si="10"/>
         <v>1369.4547744732872</v>
       </c>
-      <c r="AC10" s="89">
+      <c r="AC10" s="85">
         <f t="shared" si="0"/>
         <v>211.54522552671278</v>
       </c>
-      <c r="AD10" s="94" t="s">
+      <c r="AD10" s="90" t="s">
         <v>30</v>
       </c>
       <c r="AE10" s="4"/>
@@ -2419,11 +2419,11 @@
         <f t="shared" si="10"/>
         <v>2202.2302206989007</v>
       </c>
-      <c r="AC11" s="89">
+      <c r="AC11" s="85">
         <f t="shared" si="0"/>
         <v>344.76977930109933</v>
       </c>
-      <c r="AD11" s="94" t="s">
+      <c r="AD11" s="90" t="s">
         <v>30</v>
       </c>
       <c r="AE11" s="4"/>
@@ -2519,11 +2519,11 @@
         <f t="shared" si="10"/>
         <v>683.89978255037113</v>
       </c>
-      <c r="AC12" s="89">
+      <c r="AC12" s="85">
         <f t="shared" si="0"/>
         <v>282.10021744962887</v>
       </c>
-      <c r="AD12" s="94" t="s">
+      <c r="AD12" s="90" t="s">
         <v>30</v>
       </c>
       <c r="AE12" s="4"/>
@@ -2613,11 +2613,11 @@
         <f t="shared" si="10"/>
         <v>1293.3476097964581</v>
       </c>
-      <c r="AC13" s="89">
+      <c r="AC13" s="85">
         <f t="shared" si="0"/>
         <v>638.65239020354193</v>
       </c>
-      <c r="AD13" s="94" t="s">
+      <c r="AD13" s="90" t="s">
         <v>30</v>
       </c>
       <c r="AE13" s="4"/>
@@ -2707,11 +2707,11 @@
         <f t="shared" si="10"/>
         <v>2331.3616035848409</v>
       </c>
-      <c r="AC14" s="89">
+      <c r="AC14" s="85">
         <f t="shared" si="0"/>
         <v>566.63839641515915</v>
       </c>
-      <c r="AD14" s="94" t="s">
+      <c r="AD14" s="90" t="s">
         <v>30</v>
       </c>
       <c r="AE14" s="4"/>
@@ -2807,11 +2807,11 @@
         <f t="shared" si="10"/>
         <v>1316.9067952590854</v>
       </c>
-      <c r="AC15" s="89">
+      <c r="AC15" s="85">
         <f t="shared" si="0"/>
         <v>615.09320474091464</v>
       </c>
-      <c r="AD15" s="94" t="s">
+      <c r="AD15" s="90" t="s">
         <v>30</v>
       </c>
       <c r="AE15" s="4"/>
@@ -2905,7 +2905,7 @@
         <f t="shared" si="0"/>
         <v>954.90309757408295</v>
       </c>
-      <c r="AD16" s="90" t="s">
+      <c r="AD16" s="86" t="s">
         <v>30</v>
       </c>
       <c r="AE16" s="4"/>
@@ -3006,7 +3006,9 @@
       <c r="AF17" s="5"/>
     </row>
     <row r="18" spans="2:32" s="1" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B18" s="18"/>
+      <c r="B18" s="18">
+        <v>5</v>
+      </c>
       <c r="C18" s="32"/>
       <c r="D18" s="33"/>
       <c r="E18" s="32"/>
@@ -3674,31 +3676,31 @@
     </row>
     <row r="39" spans="1:30" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="48"/>
-      <c r="B39" s="80"/>
-      <c r="C39" s="80"/>
-      <c r="D39" s="80"/>
-      <c r="E39" s="80"/>
-      <c r="F39" s="80"/>
-      <c r="G39" s="80"/>
-      <c r="H39" s="80"/>
-      <c r="I39" s="80"/>
-      <c r="J39" s="80"/>
-      <c r="K39" s="80"/>
-      <c r="L39" s="80"/>
-      <c r="M39" s="80"/>
-      <c r="N39" s="80"/>
-      <c r="O39" s="80"/>
-      <c r="P39" s="80"/>
-      <c r="Q39" s="80"/>
-      <c r="R39" s="80"/>
-      <c r="S39" s="80"/>
-      <c r="T39" s="80"/>
-      <c r="U39" s="80"/>
-      <c r="V39" s="80"/>
-      <c r="W39" s="80"/>
-      <c r="X39" s="80"/>
-      <c r="Y39" s="80"/>
-      <c r="Z39" s="80"/>
+      <c r="B39" s="93"/>
+      <c r="C39" s="93"/>
+      <c r="D39" s="93"/>
+      <c r="E39" s="93"/>
+      <c r="F39" s="93"/>
+      <c r="G39" s="93"/>
+      <c r="H39" s="93"/>
+      <c r="I39" s="93"/>
+      <c r="J39" s="93"/>
+      <c r="K39" s="93"/>
+      <c r="L39" s="93"/>
+      <c r="M39" s="93"/>
+      <c r="N39" s="93"/>
+      <c r="O39" s="93"/>
+      <c r="P39" s="93"/>
+      <c r="Q39" s="93"/>
+      <c r="R39" s="93"/>
+      <c r="S39" s="93"/>
+      <c r="T39" s="93"/>
+      <c r="U39" s="93"/>
+      <c r="V39" s="93"/>
+      <c r="W39" s="93"/>
+      <c r="X39" s="93"/>
+      <c r="Y39" s="93"/>
+      <c r="Z39" s="93"/>
       <c r="AA39" s="55"/>
       <c r="AB39" s="55"/>
       <c r="AC39" s="55"/>
@@ -3706,33 +3708,33 @@
     </row>
     <row r="40" spans="1:30" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="48"/>
-      <c r="B40" s="80"/>
-      <c r="C40" s="80"/>
-      <c r="D40" s="80"/>
-      <c r="E40" s="80"/>
-      <c r="F40" s="80"/>
-      <c r="G40" s="80"/>
-      <c r="H40" s="80"/>
-      <c r="I40" s="80"/>
-      <c r="J40" s="80"/>
-      <c r="K40" s="80"/>
-      <c r="L40" s="80"/>
-      <c r="M40" s="80"/>
-      <c r="N40" s="80"/>
-      <c r="O40" s="80"/>
-      <c r="P40" s="80"/>
-      <c r="Q40" s="80"/>
-      <c r="R40" s="80"/>
-      <c r="S40" s="80"/>
-      <c r="T40" s="80"/>
-      <c r="U40" s="80"/>
-      <c r="V40" s="80"/>
-      <c r="W40" s="80"/>
-      <c r="X40" s="80"/>
-      <c r="Y40" s="80"/>
-      <c r="Z40" s="80"/>
-      <c r="AA40" s="80"/>
-      <c r="AB40" s="80"/>
+      <c r="B40" s="93"/>
+      <c r="C40" s="93"/>
+      <c r="D40" s="93"/>
+      <c r="E40" s="93"/>
+      <c r="F40" s="93"/>
+      <c r="G40" s="93"/>
+      <c r="H40" s="93"/>
+      <c r="I40" s="93"/>
+      <c r="J40" s="93"/>
+      <c r="K40" s="93"/>
+      <c r="L40" s="93"/>
+      <c r="M40" s="93"/>
+      <c r="N40" s="93"/>
+      <c r="O40" s="93"/>
+      <c r="P40" s="93"/>
+      <c r="Q40" s="93"/>
+      <c r="R40" s="93"/>
+      <c r="S40" s="93"/>
+      <c r="T40" s="93"/>
+      <c r="U40" s="93"/>
+      <c r="V40" s="93"/>
+      <c r="W40" s="93"/>
+      <c r="X40" s="93"/>
+      <c r="Y40" s="93"/>
+      <c r="Z40" s="93"/>
+      <c r="AA40" s="93"/>
+      <c r="AB40" s="93"/>
       <c r="AC40" s="56"/>
       <c r="AD40" s="48"/>
     </row>
@@ -3770,31 +3772,31 @@
     </row>
     <row r="42" spans="1:30" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="48"/>
-      <c r="B42" s="80"/>
-      <c r="C42" s="80"/>
-      <c r="D42" s="80"/>
-      <c r="E42" s="80"/>
-      <c r="F42" s="80"/>
-      <c r="G42" s="80"/>
-      <c r="H42" s="80"/>
-      <c r="I42" s="80"/>
-      <c r="J42" s="80"/>
-      <c r="K42" s="80"/>
-      <c r="L42" s="80"/>
-      <c r="M42" s="80"/>
-      <c r="N42" s="80"/>
-      <c r="O42" s="80"/>
-      <c r="P42" s="80"/>
-      <c r="Q42" s="80"/>
-      <c r="R42" s="80"/>
-      <c r="S42" s="80"/>
-      <c r="T42" s="80"/>
-      <c r="U42" s="80"/>
-      <c r="V42" s="80"/>
-      <c r="W42" s="80"/>
-      <c r="X42" s="80"/>
-      <c r="Y42" s="80"/>
-      <c r="Z42" s="80"/>
+      <c r="B42" s="93"/>
+      <c r="C42" s="93"/>
+      <c r="D42" s="93"/>
+      <c r="E42" s="93"/>
+      <c r="F42" s="93"/>
+      <c r="G42" s="93"/>
+      <c r="H42" s="93"/>
+      <c r="I42" s="93"/>
+      <c r="J42" s="93"/>
+      <c r="K42" s="93"/>
+      <c r="L42" s="93"/>
+      <c r="M42" s="93"/>
+      <c r="N42" s="93"/>
+      <c r="O42" s="93"/>
+      <c r="P42" s="93"/>
+      <c r="Q42" s="93"/>
+      <c r="R42" s="93"/>
+      <c r="S42" s="93"/>
+      <c r="T42" s="93"/>
+      <c r="U42" s="93"/>
+      <c r="V42" s="93"/>
+      <c r="W42" s="93"/>
+      <c r="X42" s="93"/>
+      <c r="Y42" s="93"/>
+      <c r="Z42" s="93"/>
       <c r="AA42" s="55"/>
       <c r="AB42" s="55"/>
       <c r="AC42" s="55"/>
@@ -3834,31 +3836,31 @@
     </row>
     <row r="44" spans="1:30" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="48"/>
-      <c r="B44" s="80"/>
-      <c r="C44" s="80"/>
-      <c r="D44" s="80"/>
-      <c r="E44" s="80"/>
-      <c r="F44" s="80"/>
-      <c r="G44" s="80"/>
-      <c r="H44" s="80"/>
-      <c r="I44" s="80"/>
-      <c r="J44" s="80"/>
-      <c r="K44" s="80"/>
-      <c r="L44" s="80"/>
-      <c r="M44" s="80"/>
-      <c r="N44" s="80"/>
-      <c r="O44" s="80"/>
-      <c r="P44" s="80"/>
-      <c r="Q44" s="80"/>
-      <c r="R44" s="80"/>
-      <c r="S44" s="80"/>
-      <c r="T44" s="80"/>
-      <c r="U44" s="80"/>
-      <c r="V44" s="80"/>
-      <c r="W44" s="80"/>
-      <c r="X44" s="80"/>
-      <c r="Y44" s="80"/>
-      <c r="Z44" s="80"/>
+      <c r="B44" s="93"/>
+      <c r="C44" s="93"/>
+      <c r="D44" s="93"/>
+      <c r="E44" s="93"/>
+      <c r="F44" s="93"/>
+      <c r="G44" s="93"/>
+      <c r="H44" s="93"/>
+      <c r="I44" s="93"/>
+      <c r="J44" s="93"/>
+      <c r="K44" s="93"/>
+      <c r="L44" s="93"/>
+      <c r="M44" s="93"/>
+      <c r="N44" s="93"/>
+      <c r="O44" s="93"/>
+      <c r="P44" s="93"/>
+      <c r="Q44" s="93"/>
+      <c r="R44" s="93"/>
+      <c r="S44" s="93"/>
+      <c r="T44" s="93"/>
+      <c r="U44" s="93"/>
+      <c r="V44" s="93"/>
+      <c r="W44" s="93"/>
+      <c r="X44" s="93"/>
+      <c r="Y44" s="93"/>
+      <c r="Z44" s="93"/>
       <c r="AA44" s="55"/>
       <c r="AB44" s="55"/>
       <c r="AC44" s="55"/>
@@ -3898,31 +3900,31 @@
     </row>
     <row r="46" spans="1:30" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="48"/>
-      <c r="B46" s="80"/>
-      <c r="C46" s="80"/>
-      <c r="D46" s="80"/>
-      <c r="E46" s="80"/>
-      <c r="F46" s="80"/>
-      <c r="G46" s="80"/>
-      <c r="H46" s="80"/>
-      <c r="I46" s="80"/>
-      <c r="J46" s="80"/>
-      <c r="K46" s="80"/>
-      <c r="L46" s="80"/>
-      <c r="M46" s="80"/>
-      <c r="N46" s="80"/>
-      <c r="O46" s="80"/>
-      <c r="P46" s="80"/>
-      <c r="Q46" s="80"/>
-      <c r="R46" s="80"/>
-      <c r="S46" s="80"/>
-      <c r="T46" s="80"/>
-      <c r="U46" s="80"/>
-      <c r="V46" s="80"/>
-      <c r="W46" s="80"/>
-      <c r="X46" s="80"/>
-      <c r="Y46" s="80"/>
-      <c r="Z46" s="80"/>
+      <c r="B46" s="93"/>
+      <c r="C46" s="93"/>
+      <c r="D46" s="93"/>
+      <c r="E46" s="93"/>
+      <c r="F46" s="93"/>
+      <c r="G46" s="93"/>
+      <c r="H46" s="93"/>
+      <c r="I46" s="93"/>
+      <c r="J46" s="93"/>
+      <c r="K46" s="93"/>
+      <c r="L46" s="93"/>
+      <c r="M46" s="93"/>
+      <c r="N46" s="93"/>
+      <c r="O46" s="93"/>
+      <c r="P46" s="93"/>
+      <c r="Q46" s="93"/>
+      <c r="R46" s="93"/>
+      <c r="S46" s="93"/>
+      <c r="T46" s="93"/>
+      <c r="U46" s="93"/>
+      <c r="V46" s="93"/>
+      <c r="W46" s="93"/>
+      <c r="X46" s="93"/>
+      <c r="Y46" s="93"/>
+      <c r="Z46" s="93"/>
       <c r="AA46" s="55"/>
       <c r="AB46" s="55"/>
       <c r="AC46" s="55"/>
@@ -3962,31 +3964,31 @@
     </row>
     <row r="48" spans="1:30" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="48"/>
-      <c r="B48" s="80"/>
-      <c r="C48" s="80"/>
-      <c r="D48" s="80"/>
-      <c r="E48" s="80"/>
-      <c r="F48" s="80"/>
-      <c r="G48" s="80"/>
-      <c r="H48" s="80"/>
-      <c r="I48" s="80"/>
-      <c r="J48" s="80"/>
-      <c r="K48" s="80"/>
-      <c r="L48" s="80"/>
-      <c r="M48" s="80"/>
-      <c r="N48" s="80"/>
-      <c r="O48" s="80"/>
-      <c r="P48" s="80"/>
-      <c r="Q48" s="80"/>
-      <c r="R48" s="80"/>
-      <c r="S48" s="80"/>
-      <c r="T48" s="80"/>
-      <c r="U48" s="80"/>
-      <c r="V48" s="80"/>
-      <c r="W48" s="80"/>
-      <c r="X48" s="80"/>
-      <c r="Y48" s="80"/>
-      <c r="Z48" s="80"/>
+      <c r="B48" s="93"/>
+      <c r="C48" s="93"/>
+      <c r="D48" s="93"/>
+      <c r="E48" s="93"/>
+      <c r="F48" s="93"/>
+      <c r="G48" s="93"/>
+      <c r="H48" s="93"/>
+      <c r="I48" s="93"/>
+      <c r="J48" s="93"/>
+      <c r="K48" s="93"/>
+      <c r="L48" s="93"/>
+      <c r="M48" s="93"/>
+      <c r="N48" s="93"/>
+      <c r="O48" s="93"/>
+      <c r="P48" s="93"/>
+      <c r="Q48" s="93"/>
+      <c r="R48" s="93"/>
+      <c r="S48" s="93"/>
+      <c r="T48" s="93"/>
+      <c r="U48" s="93"/>
+      <c r="V48" s="93"/>
+      <c r="W48" s="93"/>
+      <c r="X48" s="93"/>
+      <c r="Y48" s="93"/>
+      <c r="Z48" s="93"/>
       <c r="AA48" s="48"/>
       <c r="AB48" s="48"/>
       <c r="AC48" s="48"/>
@@ -4026,31 +4028,31 @@
     </row>
     <row r="50" spans="1:30" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="48"/>
-      <c r="B50" s="81"/>
-      <c r="C50" s="81"/>
-      <c r="D50" s="81"/>
-      <c r="E50" s="81"/>
-      <c r="F50" s="81"/>
-      <c r="G50" s="81"/>
-      <c r="H50" s="81"/>
-      <c r="I50" s="81"/>
-      <c r="J50" s="81"/>
-      <c r="K50" s="81"/>
-      <c r="L50" s="81"/>
-      <c r="M50" s="81"/>
-      <c r="N50" s="81"/>
-      <c r="O50" s="81"/>
-      <c r="P50" s="81"/>
-      <c r="Q50" s="81"/>
-      <c r="R50" s="81"/>
-      <c r="S50" s="81"/>
-      <c r="T50" s="81"/>
-      <c r="U50" s="81"/>
-      <c r="V50" s="81"/>
-      <c r="W50" s="81"/>
-      <c r="X50" s="81"/>
-      <c r="Y50" s="81"/>
-      <c r="Z50" s="81"/>
+      <c r="B50" s="94"/>
+      <c r="C50" s="94"/>
+      <c r="D50" s="94"/>
+      <c r="E50" s="94"/>
+      <c r="F50" s="94"/>
+      <c r="G50" s="94"/>
+      <c r="H50" s="94"/>
+      <c r="I50" s="94"/>
+      <c r="J50" s="94"/>
+      <c r="K50" s="94"/>
+      <c r="L50" s="94"/>
+      <c r="M50" s="94"/>
+      <c r="N50" s="94"/>
+      <c r="O50" s="94"/>
+      <c r="P50" s="94"/>
+      <c r="Q50" s="94"/>
+      <c r="R50" s="94"/>
+      <c r="S50" s="94"/>
+      <c r="T50" s="94"/>
+      <c r="U50" s="94"/>
+      <c r="V50" s="94"/>
+      <c r="W50" s="94"/>
+      <c r="X50" s="94"/>
+      <c r="Y50" s="94"/>
+      <c r="Z50" s="94"/>
       <c r="AA50" s="48"/>
       <c r="AB50" s="48"/>
       <c r="AC50" s="48"/>
@@ -4058,31 +4060,31 @@
     </row>
     <row r="51" spans="1:30" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="48"/>
-      <c r="B51" s="83"/>
-      <c r="C51" s="83"/>
-      <c r="D51" s="83"/>
-      <c r="E51" s="83"/>
-      <c r="F51" s="83"/>
-      <c r="G51" s="83"/>
-      <c r="H51" s="83"/>
-      <c r="I51" s="83"/>
-      <c r="J51" s="83"/>
-      <c r="K51" s="83"/>
-      <c r="L51" s="83"/>
-      <c r="M51" s="83"/>
-      <c r="N51" s="83"/>
-      <c r="O51" s="83"/>
-      <c r="P51" s="83"/>
-      <c r="Q51" s="83"/>
-      <c r="R51" s="83"/>
-      <c r="S51" s="83"/>
-      <c r="T51" s="83"/>
-      <c r="U51" s="83"/>
-      <c r="V51" s="83"/>
-      <c r="W51" s="83"/>
-      <c r="X51" s="83"/>
-      <c r="Y51" s="83"/>
-      <c r="Z51" s="83"/>
+      <c r="B51" s="91"/>
+      <c r="C51" s="91"/>
+      <c r="D51" s="91"/>
+      <c r="E51" s="91"/>
+      <c r="F51" s="91"/>
+      <c r="G51" s="91"/>
+      <c r="H51" s="91"/>
+      <c r="I51" s="91"/>
+      <c r="J51" s="91"/>
+      <c r="K51" s="91"/>
+      <c r="L51" s="91"/>
+      <c r="M51" s="91"/>
+      <c r="N51" s="91"/>
+      <c r="O51" s="91"/>
+      <c r="P51" s="91"/>
+      <c r="Q51" s="91"/>
+      <c r="R51" s="91"/>
+      <c r="S51" s="91"/>
+      <c r="T51" s="91"/>
+      <c r="U51" s="91"/>
+      <c r="V51" s="91"/>
+      <c r="W51" s="91"/>
+      <c r="X51" s="91"/>
+      <c r="Y51" s="91"/>
+      <c r="Z51" s="91"/>
       <c r="AA51" s="48"/>
       <c r="AB51" s="48"/>
       <c r="AC51" s="48"/>
@@ -4090,31 +4092,31 @@
     </row>
     <row r="52" spans="1:30" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" s="48"/>
-      <c r="B52" s="83"/>
-      <c r="C52" s="83"/>
-      <c r="D52" s="83"/>
-      <c r="E52" s="83"/>
-      <c r="F52" s="83"/>
-      <c r="G52" s="83"/>
-      <c r="H52" s="83"/>
-      <c r="I52" s="83"/>
-      <c r="J52" s="83"/>
-      <c r="K52" s="83"/>
-      <c r="L52" s="83"/>
-      <c r="M52" s="83"/>
-      <c r="N52" s="83"/>
-      <c r="O52" s="83"/>
-      <c r="P52" s="83"/>
-      <c r="Q52" s="83"/>
-      <c r="R52" s="83"/>
-      <c r="S52" s="83"/>
-      <c r="T52" s="83"/>
-      <c r="U52" s="83"/>
-      <c r="V52" s="83"/>
-      <c r="W52" s="83"/>
-      <c r="X52" s="83"/>
-      <c r="Y52" s="83"/>
-      <c r="Z52" s="83"/>
+      <c r="B52" s="91"/>
+      <c r="C52" s="91"/>
+      <c r="D52" s="91"/>
+      <c r="E52" s="91"/>
+      <c r="F52" s="91"/>
+      <c r="G52" s="91"/>
+      <c r="H52" s="91"/>
+      <c r="I52" s="91"/>
+      <c r="J52" s="91"/>
+      <c r="K52" s="91"/>
+      <c r="L52" s="91"/>
+      <c r="M52" s="91"/>
+      <c r="N52" s="91"/>
+      <c r="O52" s="91"/>
+      <c r="P52" s="91"/>
+      <c r="Q52" s="91"/>
+      <c r="R52" s="91"/>
+      <c r="S52" s="91"/>
+      <c r="T52" s="91"/>
+      <c r="U52" s="91"/>
+      <c r="V52" s="91"/>
+      <c r="W52" s="91"/>
+      <c r="X52" s="91"/>
+      <c r="Y52" s="91"/>
+      <c r="Z52" s="91"/>
       <c r="AA52" s="48"/>
       <c r="AB52" s="48"/>
       <c r="AC52" s="48"/>
@@ -4122,31 +4124,31 @@
     </row>
     <row r="53" spans="1:30" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A53" s="48"/>
-      <c r="B53" s="83"/>
-      <c r="C53" s="83"/>
-      <c r="D53" s="83"/>
-      <c r="E53" s="83"/>
-      <c r="F53" s="83"/>
-      <c r="G53" s="83"/>
-      <c r="H53" s="83"/>
-      <c r="I53" s="83"/>
-      <c r="J53" s="83"/>
-      <c r="K53" s="83"/>
-      <c r="L53" s="83"/>
-      <c r="M53" s="83"/>
-      <c r="N53" s="83"/>
-      <c r="O53" s="83"/>
-      <c r="P53" s="83"/>
-      <c r="Q53" s="83"/>
-      <c r="R53" s="83"/>
-      <c r="S53" s="83"/>
-      <c r="T53" s="83"/>
-      <c r="U53" s="83"/>
-      <c r="V53" s="83"/>
-      <c r="W53" s="83"/>
-      <c r="X53" s="83"/>
-      <c r="Y53" s="83"/>
-      <c r="Z53" s="83"/>
+      <c r="B53" s="91"/>
+      <c r="C53" s="91"/>
+      <c r="D53" s="91"/>
+      <c r="E53" s="91"/>
+      <c r="F53" s="91"/>
+      <c r="G53" s="91"/>
+      <c r="H53" s="91"/>
+      <c r="I53" s="91"/>
+      <c r="J53" s="91"/>
+      <c r="K53" s="91"/>
+      <c r="L53" s="91"/>
+      <c r="M53" s="91"/>
+      <c r="N53" s="91"/>
+      <c r="O53" s="91"/>
+      <c r="P53" s="91"/>
+      <c r="Q53" s="91"/>
+      <c r="R53" s="91"/>
+      <c r="S53" s="91"/>
+      <c r="T53" s="91"/>
+      <c r="U53" s="91"/>
+      <c r="V53" s="91"/>
+      <c r="W53" s="91"/>
+      <c r="X53" s="91"/>
+      <c r="Y53" s="91"/>
+      <c r="Z53" s="91"/>
       <c r="AA53" s="48"/>
       <c r="AB53" s="48"/>
       <c r="AC53" s="48"/>
@@ -4154,31 +4156,31 @@
     </row>
     <row r="54" spans="1:30" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A54" s="48"/>
-      <c r="B54" s="83"/>
-      <c r="C54" s="83"/>
-      <c r="D54" s="83"/>
-      <c r="E54" s="83"/>
-      <c r="F54" s="83"/>
-      <c r="G54" s="83"/>
-      <c r="H54" s="83"/>
-      <c r="I54" s="83"/>
-      <c r="J54" s="83"/>
-      <c r="K54" s="83"/>
-      <c r="L54" s="83"/>
-      <c r="M54" s="83"/>
-      <c r="N54" s="83"/>
-      <c r="O54" s="83"/>
-      <c r="P54" s="83"/>
-      <c r="Q54" s="83"/>
-      <c r="R54" s="83"/>
-      <c r="S54" s="83"/>
-      <c r="T54" s="83"/>
-      <c r="U54" s="83"/>
-      <c r="V54" s="83"/>
-      <c r="W54" s="83"/>
-      <c r="X54" s="83"/>
-      <c r="Y54" s="83"/>
-      <c r="Z54" s="83"/>
+      <c r="B54" s="91"/>
+      <c r="C54" s="91"/>
+      <c r="D54" s="91"/>
+      <c r="E54" s="91"/>
+      <c r="F54" s="91"/>
+      <c r="G54" s="91"/>
+      <c r="H54" s="91"/>
+      <c r="I54" s="91"/>
+      <c r="J54" s="91"/>
+      <c r="K54" s="91"/>
+      <c r="L54" s="91"/>
+      <c r="M54" s="91"/>
+      <c r="N54" s="91"/>
+      <c r="O54" s="91"/>
+      <c r="P54" s="91"/>
+      <c r="Q54" s="91"/>
+      <c r="R54" s="91"/>
+      <c r="S54" s="91"/>
+      <c r="T54" s="91"/>
+      <c r="U54" s="91"/>
+      <c r="V54" s="91"/>
+      <c r="W54" s="91"/>
+      <c r="X54" s="91"/>
+      <c r="Y54" s="91"/>
+      <c r="Z54" s="91"/>
       <c r="AA54" s="48"/>
       <c r="AB54" s="48"/>
       <c r="AC54" s="48"/>
@@ -4186,31 +4188,31 @@
     </row>
     <row r="55" spans="1:30" customFormat="1" ht="50.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A55" s="48"/>
-      <c r="B55" s="83"/>
-      <c r="C55" s="83"/>
-      <c r="D55" s="83"/>
-      <c r="E55" s="83"/>
-      <c r="F55" s="83"/>
-      <c r="G55" s="83"/>
-      <c r="H55" s="83"/>
-      <c r="I55" s="83"/>
-      <c r="J55" s="83"/>
-      <c r="K55" s="83"/>
-      <c r="L55" s="83"/>
-      <c r="M55" s="83"/>
-      <c r="N55" s="83"/>
-      <c r="O55" s="83"/>
-      <c r="P55" s="83"/>
-      <c r="Q55" s="83"/>
-      <c r="R55" s="83"/>
-      <c r="S55" s="83"/>
-      <c r="T55" s="83"/>
-      <c r="U55" s="83"/>
-      <c r="V55" s="83"/>
-      <c r="W55" s="83"/>
-      <c r="X55" s="83"/>
-      <c r="Y55" s="83"/>
-      <c r="Z55" s="83"/>
+      <c r="B55" s="91"/>
+      <c r="C55" s="91"/>
+      <c r="D55" s="91"/>
+      <c r="E55" s="91"/>
+      <c r="F55" s="91"/>
+      <c r="G55" s="91"/>
+      <c r="H55" s="91"/>
+      <c r="I55" s="91"/>
+      <c r="J55" s="91"/>
+      <c r="K55" s="91"/>
+      <c r="L55" s="91"/>
+      <c r="M55" s="91"/>
+      <c r="N55" s="91"/>
+      <c r="O55" s="91"/>
+      <c r="P55" s="91"/>
+      <c r="Q55" s="91"/>
+      <c r="R55" s="91"/>
+      <c r="S55" s="91"/>
+      <c r="T55" s="91"/>
+      <c r="U55" s="91"/>
+      <c r="V55" s="91"/>
+      <c r="W55" s="91"/>
+      <c r="X55" s="91"/>
+      <c r="Y55" s="91"/>
+      <c r="Z55" s="91"/>
       <c r="AA55" s="48"/>
       <c r="AB55" s="48"/>
       <c r="AC55" s="48"/>
@@ -4218,31 +4220,31 @@
     </row>
     <row r="56" spans="1:30" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A56" s="48"/>
-      <c r="B56" s="83"/>
-      <c r="C56" s="83"/>
-      <c r="D56" s="83"/>
-      <c r="E56" s="83"/>
-      <c r="F56" s="83"/>
-      <c r="G56" s="83"/>
-      <c r="H56" s="83"/>
-      <c r="I56" s="83"/>
-      <c r="J56" s="83"/>
-      <c r="K56" s="83"/>
-      <c r="L56" s="83"/>
-      <c r="M56" s="83"/>
-      <c r="N56" s="83"/>
-      <c r="O56" s="83"/>
-      <c r="P56" s="83"/>
-      <c r="Q56" s="83"/>
-      <c r="R56" s="83"/>
-      <c r="S56" s="83"/>
-      <c r="T56" s="83"/>
-      <c r="U56" s="83"/>
-      <c r="V56" s="83"/>
-      <c r="W56" s="83"/>
-      <c r="X56" s="83"/>
-      <c r="Y56" s="83"/>
-      <c r="Z56" s="83"/>
+      <c r="B56" s="91"/>
+      <c r="C56" s="91"/>
+      <c r="D56" s="91"/>
+      <c r="E56" s="91"/>
+      <c r="F56" s="91"/>
+      <c r="G56" s="91"/>
+      <c r="H56" s="91"/>
+      <c r="I56" s="91"/>
+      <c r="J56" s="91"/>
+      <c r="K56" s="91"/>
+      <c r="L56" s="91"/>
+      <c r="M56" s="91"/>
+      <c r="N56" s="91"/>
+      <c r="O56" s="91"/>
+      <c r="P56" s="91"/>
+      <c r="Q56" s="91"/>
+      <c r="R56" s="91"/>
+      <c r="S56" s="91"/>
+      <c r="T56" s="91"/>
+      <c r="U56" s="91"/>
+      <c r="V56" s="91"/>
+      <c r="W56" s="91"/>
+      <c r="X56" s="91"/>
+      <c r="Y56" s="91"/>
+      <c r="Z56" s="91"/>
       <c r="AA56" s="48"/>
       <c r="AB56" s="48"/>
       <c r="AC56" s="48"/>
@@ -4282,31 +4284,31 @@
     </row>
     <row r="58" spans="1:30" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A58" s="48"/>
-      <c r="B58" s="80"/>
-      <c r="C58" s="80"/>
-      <c r="D58" s="80"/>
-      <c r="E58" s="80"/>
-      <c r="F58" s="80"/>
-      <c r="G58" s="80"/>
-      <c r="H58" s="80"/>
-      <c r="I58" s="80"/>
-      <c r="J58" s="80"/>
-      <c r="K58" s="80"/>
-      <c r="L58" s="80"/>
-      <c r="M58" s="80"/>
-      <c r="N58" s="80"/>
-      <c r="O58" s="80"/>
-      <c r="P58" s="80"/>
-      <c r="Q58" s="80"/>
-      <c r="R58" s="80"/>
-      <c r="S58" s="80"/>
-      <c r="T58" s="80"/>
-      <c r="U58" s="80"/>
-      <c r="V58" s="80"/>
-      <c r="W58" s="80"/>
-      <c r="X58" s="80"/>
-      <c r="Y58" s="80"/>
-      <c r="Z58" s="80"/>
+      <c r="B58" s="93"/>
+      <c r="C58" s="93"/>
+      <c r="D58" s="93"/>
+      <c r="E58" s="93"/>
+      <c r="F58" s="93"/>
+      <c r="G58" s="93"/>
+      <c r="H58" s="93"/>
+      <c r="I58" s="93"/>
+      <c r="J58" s="93"/>
+      <c r="K58" s="93"/>
+      <c r="L58" s="93"/>
+      <c r="M58" s="93"/>
+      <c r="N58" s="93"/>
+      <c r="O58" s="93"/>
+      <c r="P58" s="93"/>
+      <c r="Q58" s="93"/>
+      <c r="R58" s="93"/>
+      <c r="S58" s="93"/>
+      <c r="T58" s="93"/>
+      <c r="U58" s="93"/>
+      <c r="V58" s="93"/>
+      <c r="W58" s="93"/>
+      <c r="X58" s="93"/>
+      <c r="Y58" s="93"/>
+      <c r="Z58" s="93"/>
       <c r="AA58" s="48"/>
       <c r="AB58" s="48"/>
       <c r="AC58" s="48"/>
@@ -4346,31 +4348,31 @@
     </row>
     <row r="60" spans="1:30" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A60" s="48"/>
-      <c r="B60" s="80"/>
-      <c r="C60" s="80"/>
-      <c r="D60" s="80"/>
-      <c r="E60" s="80"/>
-      <c r="F60" s="80"/>
-      <c r="G60" s="80"/>
-      <c r="H60" s="80"/>
-      <c r="I60" s="80"/>
-      <c r="J60" s="80"/>
-      <c r="K60" s="80"/>
-      <c r="L60" s="80"/>
-      <c r="M60" s="80"/>
-      <c r="N60" s="80"/>
-      <c r="O60" s="80"/>
-      <c r="P60" s="80"/>
-      <c r="Q60" s="80"/>
-      <c r="R60" s="80"/>
-      <c r="S60" s="80"/>
-      <c r="T60" s="80"/>
-      <c r="U60" s="80"/>
-      <c r="V60" s="80"/>
-      <c r="W60" s="80"/>
-      <c r="X60" s="80"/>
-      <c r="Y60" s="80"/>
-      <c r="Z60" s="80"/>
+      <c r="B60" s="93"/>
+      <c r="C60" s="93"/>
+      <c r="D60" s="93"/>
+      <c r="E60" s="93"/>
+      <c r="F60" s="93"/>
+      <c r="G60" s="93"/>
+      <c r="H60" s="93"/>
+      <c r="I60" s="93"/>
+      <c r="J60" s="93"/>
+      <c r="K60" s="93"/>
+      <c r="L60" s="93"/>
+      <c r="M60" s="93"/>
+      <c r="N60" s="93"/>
+      <c r="O60" s="93"/>
+      <c r="P60" s="93"/>
+      <c r="Q60" s="93"/>
+      <c r="R60" s="93"/>
+      <c r="S60" s="93"/>
+      <c r="T60" s="93"/>
+      <c r="U60" s="93"/>
+      <c r="V60" s="93"/>
+      <c r="W60" s="93"/>
+      <c r="X60" s="93"/>
+      <c r="Y60" s="93"/>
+      <c r="Z60" s="93"/>
       <c r="AA60" s="48"/>
       <c r="AB60" s="48"/>
       <c r="AC60" s="48"/>
@@ -4410,31 +4412,31 @@
     </row>
     <row r="62" spans="1:30" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A62" s="48"/>
-      <c r="B62" s="80"/>
-      <c r="C62" s="80"/>
-      <c r="D62" s="80"/>
-      <c r="E62" s="80"/>
-      <c r="F62" s="80"/>
-      <c r="G62" s="80"/>
-      <c r="H62" s="80"/>
-      <c r="I62" s="80"/>
-      <c r="J62" s="80"/>
-      <c r="K62" s="80"/>
-      <c r="L62" s="80"/>
-      <c r="M62" s="80"/>
-      <c r="N62" s="80"/>
-      <c r="O62" s="80"/>
-      <c r="P62" s="80"/>
-      <c r="Q62" s="80"/>
-      <c r="R62" s="80"/>
-      <c r="S62" s="80"/>
-      <c r="T62" s="80"/>
-      <c r="U62" s="80"/>
-      <c r="V62" s="80"/>
-      <c r="W62" s="80"/>
-      <c r="X62" s="80"/>
-      <c r="Y62" s="80"/>
-      <c r="Z62" s="80"/>
+      <c r="B62" s="93"/>
+      <c r="C62" s="93"/>
+      <c r="D62" s="93"/>
+      <c r="E62" s="93"/>
+      <c r="F62" s="93"/>
+      <c r="G62" s="93"/>
+      <c r="H62" s="93"/>
+      <c r="I62" s="93"/>
+      <c r="J62" s="93"/>
+      <c r="K62" s="93"/>
+      <c r="L62" s="93"/>
+      <c r="M62" s="93"/>
+      <c r="N62" s="93"/>
+      <c r="O62" s="93"/>
+      <c r="P62" s="93"/>
+      <c r="Q62" s="93"/>
+      <c r="R62" s="93"/>
+      <c r="S62" s="93"/>
+      <c r="T62" s="93"/>
+      <c r="U62" s="93"/>
+      <c r="V62" s="93"/>
+      <c r="W62" s="93"/>
+      <c r="X62" s="93"/>
+      <c r="Y62" s="93"/>
+      <c r="Z62" s="93"/>
       <c r="AA62" s="48"/>
       <c r="AB62" s="48"/>
       <c r="AC62" s="48"/>
@@ -4474,31 +4476,31 @@
     </row>
     <row r="64" spans="1:30" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A64" s="48"/>
-      <c r="B64" s="80"/>
-      <c r="C64" s="80"/>
-      <c r="D64" s="80"/>
-      <c r="E64" s="80"/>
-      <c r="F64" s="80"/>
-      <c r="G64" s="80"/>
-      <c r="H64" s="80"/>
-      <c r="I64" s="80"/>
-      <c r="J64" s="80"/>
-      <c r="K64" s="80"/>
-      <c r="L64" s="80"/>
-      <c r="M64" s="80"/>
-      <c r="N64" s="80"/>
-      <c r="O64" s="80"/>
-      <c r="P64" s="80"/>
-      <c r="Q64" s="80"/>
-      <c r="R64" s="80"/>
-      <c r="S64" s="80"/>
-      <c r="T64" s="80"/>
-      <c r="U64" s="80"/>
-      <c r="V64" s="80"/>
-      <c r="W64" s="80"/>
-      <c r="X64" s="80"/>
-      <c r="Y64" s="80"/>
-      <c r="Z64" s="80"/>
+      <c r="B64" s="93"/>
+      <c r="C64" s="93"/>
+      <c r="D64" s="93"/>
+      <c r="E64" s="93"/>
+      <c r="F64" s="93"/>
+      <c r="G64" s="93"/>
+      <c r="H64" s="93"/>
+      <c r="I64" s="93"/>
+      <c r="J64" s="93"/>
+      <c r="K64" s="93"/>
+      <c r="L64" s="93"/>
+      <c r="M64" s="93"/>
+      <c r="N64" s="93"/>
+      <c r="O64" s="93"/>
+      <c r="P64" s="93"/>
+      <c r="Q64" s="93"/>
+      <c r="R64" s="93"/>
+      <c r="S64" s="93"/>
+      <c r="T64" s="93"/>
+      <c r="U64" s="93"/>
+      <c r="V64" s="93"/>
+      <c r="W64" s="93"/>
+      <c r="X64" s="93"/>
+      <c r="Y64" s="93"/>
+      <c r="Z64" s="93"/>
       <c r="AA64" s="48"/>
       <c r="AB64" s="48"/>
       <c r="AC64" s="48"/>
@@ -4538,31 +4540,31 @@
     </row>
     <row r="66" spans="1:30" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A66" s="48"/>
-      <c r="B66" s="82"/>
-      <c r="C66" s="82"/>
-      <c r="D66" s="82"/>
-      <c r="E66" s="82"/>
-      <c r="F66" s="82"/>
-      <c r="G66" s="82"/>
-      <c r="H66" s="82"/>
-      <c r="I66" s="82"/>
-      <c r="J66" s="82"/>
-      <c r="K66" s="82"/>
-      <c r="L66" s="82"/>
-      <c r="M66" s="82"/>
-      <c r="N66" s="82"/>
-      <c r="O66" s="82"/>
-      <c r="P66" s="82"/>
-      <c r="Q66" s="82"/>
-      <c r="R66" s="82"/>
-      <c r="S66" s="82"/>
-      <c r="T66" s="82"/>
-      <c r="U66" s="82"/>
-      <c r="V66" s="82"/>
-      <c r="W66" s="82"/>
-      <c r="X66" s="82"/>
-      <c r="Y66" s="82"/>
-      <c r="Z66" s="82"/>
+      <c r="B66" s="92"/>
+      <c r="C66" s="92"/>
+      <c r="D66" s="92"/>
+      <c r="E66" s="92"/>
+      <c r="F66" s="92"/>
+      <c r="G66" s="92"/>
+      <c r="H66" s="92"/>
+      <c r="I66" s="92"/>
+      <c r="J66" s="92"/>
+      <c r="K66" s="92"/>
+      <c r="L66" s="92"/>
+      <c r="M66" s="92"/>
+      <c r="N66" s="92"/>
+      <c r="O66" s="92"/>
+      <c r="P66" s="92"/>
+      <c r="Q66" s="92"/>
+      <c r="R66" s="92"/>
+      <c r="S66" s="92"/>
+      <c r="T66" s="92"/>
+      <c r="U66" s="92"/>
+      <c r="V66" s="92"/>
+      <c r="W66" s="92"/>
+      <c r="X66" s="92"/>
+      <c r="Y66" s="92"/>
+      <c r="Z66" s="92"/>
       <c r="AA66" s="48"/>
       <c r="AB66" s="48"/>
       <c r="AC66" s="48"/>
@@ -4762,17 +4764,6 @@
     </row>
   </sheetData>
   <mergeCells count="18">
-    <mergeCell ref="B56:Z56"/>
-    <mergeCell ref="B52:Z52"/>
-    <mergeCell ref="B53:Z53"/>
-    <mergeCell ref="B51:Z51"/>
-    <mergeCell ref="B55:Z55"/>
-    <mergeCell ref="B54:Z54"/>
-    <mergeCell ref="B66:Z66"/>
-    <mergeCell ref="B64:Z64"/>
-    <mergeCell ref="B60:Z60"/>
-    <mergeCell ref="B62:Z62"/>
-    <mergeCell ref="B58:Z58"/>
     <mergeCell ref="B48:Z48"/>
     <mergeCell ref="B44:Z44"/>
     <mergeCell ref="B50:Z50"/>
@@ -4780,6 +4771,17 @@
     <mergeCell ref="B42:Z42"/>
     <mergeCell ref="B40:AB40"/>
     <mergeCell ref="B46:Z46"/>
+    <mergeCell ref="B66:Z66"/>
+    <mergeCell ref="B64:Z64"/>
+    <mergeCell ref="B60:Z60"/>
+    <mergeCell ref="B62:Z62"/>
+    <mergeCell ref="B58:Z58"/>
+    <mergeCell ref="B56:Z56"/>
+    <mergeCell ref="B52:Z52"/>
+    <mergeCell ref="B53:Z53"/>
+    <mergeCell ref="B51:Z51"/>
+    <mergeCell ref="B55:Z55"/>
+    <mergeCell ref="B54:Z54"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>